<commit_message>
shadow casting is added to the analysis weighting
</commit_message>
<xml_diff>
--- a/Weightings analysis table excel.xlsx
+++ b/Weightings analysis table excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/serenst_tudelft_nl/Documents/spatial computing architecture/CDS-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{CE7F9EB4-7808-46B3-9007-AC2C44DFCD41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0516DBB4-4BCA-4C41-B908-98F7F6F11717}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{CE7F9EB4-7808-46B3-9007-AC2C44DFCD41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF858486-EA9B-46D5-9BB0-EB870E9BB2C1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{187382FC-803D-471F-9C3D-94C10A1BF309}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="46">
   <si>
     <t>Point X</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>0.4</t>
+  </si>
+  <si>
+    <t>Shadow casting</t>
   </si>
 </sst>
 </file>
@@ -530,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4171DEF-D904-4BB6-890A-8379EADE8FB0}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:E33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,7 +572,9 @@
       <c r="I1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="1"/>
+      <c r="J1" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -599,7 +604,9 @@
       <c r="I2" s="2">
         <v>1</v>
       </c>
-      <c r="J2" s="2"/>
+      <c r="J2" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -629,7 +636,9 @@
       <c r="I3" s="2">
         <v>1</v>
       </c>
-      <c r="J3" s="2"/>
+      <c r="J3" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -659,7 +668,9 @@
       <c r="I4" s="2">
         <v>1</v>
       </c>
-      <c r="J4" s="2"/>
+      <c r="J4" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -689,7 +700,9 @@
       <c r="I5" s="2">
         <v>0</v>
       </c>
-      <c r="J5" s="2"/>
+      <c r="J5" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -719,7 +732,9 @@
       <c r="I6" s="2">
         <v>1</v>
       </c>
-      <c r="J6" s="2"/>
+      <c r="J6" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -749,7 +764,9 @@
       <c r="I7" s="2">
         <v>1</v>
       </c>
-      <c r="J7" s="2"/>
+      <c r="J7" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -779,7 +796,9 @@
       <c r="I8" s="2">
         <v>1</v>
       </c>
-      <c r="J8" s="2"/>
+      <c r="J8" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -809,7 +828,9 @@
       <c r="I9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="J9" s="2"/>
+      <c r="J9" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -839,7 +860,9 @@
       <c r="I10" s="2">
         <v>1</v>
       </c>
-      <c r="J10" s="2"/>
+      <c r="J10" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -869,7 +892,9 @@
       <c r="I11" s="2">
         <v>1</v>
       </c>
-      <c r="J11" s="2"/>
+      <c r="J11" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -899,7 +924,9 @@
       <c r="I12" s="2">
         <v>0</v>
       </c>
-      <c r="J12" s="2"/>
+      <c r="J12" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -929,7 +956,9 @@
       <c r="I13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="J13" s="2"/>
+      <c r="J13" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -959,7 +988,9 @@
       <c r="I14" s="2">
         <v>1</v>
       </c>
-      <c r="J14" s="2"/>
+      <c r="J14" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -989,7 +1020,9 @@
       <c r="I15" s="2">
         <v>0</v>
       </c>
-      <c r="J15" s="2"/>
+      <c r="J15" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H17" t="s">
@@ -998,7 +1031,7 @@
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
-        <f>CONCATENATE(B2,",",C2,",",D2,",",E2,",",F2,",",G2,",",H2,",",I2)</f>
+        <f t="shared" ref="B20:B33" si="0">CONCATENATE(B2,",",C2,",",D2,",",E2,",",F2,",",G2,",",H2,",",I2)</f>
         <v>0,0,0,Housing_entrance,0.1,1,0.1,1</v>
       </c>
     </row>
@@ -1010,73 +1043,73 @@
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
-        <f>CONCATENATE(B4,",",C4,",",D4,",",E4,",",F4,",",G4,",",H4,",",I4)</f>
+        <f t="shared" si="0"/>
         <v>0,0,0,Student_houses,0.8,0.1,0.8,1</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
-        <f>CONCATENATE(B5,",",C5,",",D5,",",E5,",",F5,",",G5,",",H5,",",I5)</f>
+        <f t="shared" si="0"/>
         <v>0,0,0,Private_parking,0,0.8,0,0</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
-        <f>CONCATENATE(B6,",",C6,",",D6,",",E6,",",F6,",",G6,",",H6,",",I6)</f>
+        <f t="shared" si="0"/>
         <v>0,0,0,Independent_elderly_houses,0.8,0.1,0.8,1</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
-        <f>CONCATENATE(B7,",",C7,",",D7,",",E7,",",F7,",",G7,",",H7,",",I7)</f>
+        <f t="shared" si="0"/>
         <v>0,0,0,Dependent_elderly_houses,0.8,0.1,0.8,1</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
-        <f>CONCATENATE(B8,",",C8,",",D8,",",E8,",",F8,",",G8,",",H8,",",I8)</f>
+        <f t="shared" si="0"/>
         <v>0,0,0,Shared_workspaces,0.8,0.5,0.8,1</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
-        <f>CONCATENATE(B9,",",C9,",",D9,",",E9,",",F9,",",G9,",",H9,",",I9)</f>
+        <f t="shared" si="0"/>
         <v>0,0,0,Supermarket,0.2,0.9,0.2,0.5</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
-        <f>CONCATENATE(B10,",",C10,",",D10,",",E10,",",F10,",",G10,",",H10,",",I10)</f>
+        <f t="shared" si="0"/>
         <v>0,0,0,Care_center_elderly,0.7,0.7,0.7,1</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29" t="str">
-        <f>CONCATENATE(B11,",",C11,",",D11,",",E11,",",F11,",",G11,",",H11,",",I11)</f>
+        <f t="shared" si="0"/>
         <v>0,0,0,Cafe,0.6,1,0.2,1</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30" t="str">
-        <f>CONCATENATE(B12,",",C12,",",D12,",",E12,",",F12,",",G12,",",H12,",",I12)</f>
+        <f t="shared" si="0"/>
         <v>0,0,0,Loading_dock,0,1,0,0</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31" t="str">
-        <f>CONCATENATE(B13,",",C13,",",D13,",",E13,",",F13,",",G13,",",H13,",",I13)</f>
+        <f t="shared" si="0"/>
         <v>0,0,0,Gym,0.4,0.8,0.4,0.5</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
-        <f>CONCATENATE(B14,",",C14,",",D14,",",E14,",",F14,",",G14,",",H14,",",I14)</f>
+        <f t="shared" si="0"/>
         <v>0,0,0,Atrium,0.9,0,0.6,1</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
-        <f>CONCATENATE(B15,",",C15,",",D15,",",E15,",",F15,",",G15,",",H15,",",I15)</f>
+        <f t="shared" si="0"/>
         <v>0,0,0,Public_parking,0,0.8,0,0</v>
       </c>
     </row>

</xml_diff>